<commit_message>
adds "special characters". removes some logs.
</commit_message>
<xml_diff>
--- a/prep/characters8bit.xlsx
+++ b/prep/characters8bit.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tiago/Documents/github/my-patch-of-the-web/prep/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91534985-8F94-894C-9B97-823746360930}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43A43F0D-5180-5249-97C2-9C18D7959D69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-29200" yWindow="3460" windowWidth="24640" windowHeight="16500" activeTab="1" xr2:uid="{B2589E65-E8B1-364E-A64F-D98FD440D3EC}"/>
+    <workbookView xWindow="3840" yWindow="460" windowWidth="18960" windowHeight="13900" xr2:uid="{B2589E65-E8B1-364E-A64F-D98FD440D3EC}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="letters" sheetId="1" r:id="rId1"/>
     <sheet name="bar_chart" sheetId="2" r:id="rId2"/>
     <sheet name="family" sheetId="5" r:id="rId3"/>
     <sheet name="cookie" sheetId="6" r:id="rId4"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="89">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -574,27 +574,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="110">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.89996032593768116"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1214,6 +1193,27 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="2" tint="-0.89996032593768116"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
@@ -1667,8 +1667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{478EC196-EA3D-0B42-9BCE-C9EAFA77170C}">
   <dimension ref="A1:AW41"/>
   <sheetViews>
-    <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="AN38" sqref="AN38"/>
+    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="AV43" sqref="AV43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4937,7 +4937,9 @@
       <c r="AL34" s="1">
         <v>1</v>
       </c>
-      <c r="AM34" s="1"/>
+      <c r="AM34" s="1">
+        <v>1</v>
+      </c>
       <c r="AN34" s="1"/>
       <c r="AO34" s="2"/>
       <c r="AP34" s="3"/>
@@ -5026,9 +5028,7 @@
       <c r="AM35" s="4">
         <v>1</v>
       </c>
-      <c r="AN35" s="4">
-        <v>1</v>
-      </c>
+      <c r="AN35" s="4"/>
       <c r="AO35" s="5"/>
       <c r="AP35" s="6"/>
       <c r="AQ35" s="4"/>
@@ -5115,7 +5115,9 @@
       </c>
       <c r="AK36" s="4"/>
       <c r="AL36" s="4"/>
-      <c r="AM36" s="4"/>
+      <c r="AM36" s="4">
+        <v>1</v>
+      </c>
       <c r="AN36" s="4">
         <v>1</v>
       </c>
@@ -5202,10 +5204,10 @@
       <c r="AK37" s="4"/>
       <c r="AL37" s="4"/>
       <c r="AM37" s="4"/>
-      <c r="AN37" s="4"/>
-      <c r="AO37" s="5">
-        <v>1</v>
-      </c>
+      <c r="AN37" s="4">
+        <v>1</v>
+      </c>
+      <c r="AO37" s="5"/>
       <c r="AP37" s="6"/>
       <c r="AQ37" s="4"/>
       <c r="AR37" s="4"/>
@@ -5276,10 +5278,10 @@
       <c r="AK38" s="4"/>
       <c r="AL38" s="4"/>
       <c r="AM38" s="4"/>
-      <c r="AN38" s="4"/>
-      <c r="AO38" s="5">
-        <v>1</v>
-      </c>
+      <c r="AN38" s="4">
+        <v>1</v>
+      </c>
+      <c r="AO38" s="5"/>
       <c r="AP38" s="6"/>
       <c r="AQ38" s="4"/>
       <c r="AR38" s="4"/>
@@ -5353,19 +5355,35 @@
       </c>
       <c r="AK39" s="4"/>
       <c r="AL39" s="4"/>
-      <c r="AM39" s="4"/>
+      <c r="AM39" s="4">
+        <v>1</v>
+      </c>
       <c r="AN39" s="4">
         <v>1</v>
       </c>
       <c r="AO39" s="5"/>
-      <c r="AP39" s="6"/>
-      <c r="AQ39" s="4"/>
-      <c r="AR39" s="4"/>
-      <c r="AS39" s="4"/>
-      <c r="AT39" s="4"/>
+      <c r="AP39" s="6">
+        <v>1</v>
+      </c>
+      <c r="AQ39" s="4">
+        <v>1</v>
+      </c>
+      <c r="AR39" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AS39" s="4">
+        <v>1</v>
+      </c>
+      <c r="AT39" s="4">
+        <v>1</v>
+      </c>
       <c r="AU39" s="4"/>
-      <c r="AV39" s="4"/>
-      <c r="AW39" s="5"/>
+      <c r="AV39" s="4">
+        <v>1</v>
+      </c>
+      <c r="AW39" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="40" spans="1:49">
       <c r="A40" t="s">
@@ -5438,18 +5456,30 @@
       <c r="AM40" s="4">
         <v>1</v>
       </c>
-      <c r="AN40" s="4">
-        <v>1</v>
-      </c>
+      <c r="AN40" s="4"/>
       <c r="AO40" s="5"/>
-      <c r="AP40" s="6"/>
-      <c r="AQ40" s="4"/>
-      <c r="AR40" s="4"/>
-      <c r="AS40" s="4"/>
-      <c r="AT40" s="4"/>
+      <c r="AP40" s="6">
+        <v>1</v>
+      </c>
+      <c r="AQ40" s="4">
+        <v>1</v>
+      </c>
+      <c r="AR40" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AS40" s="4">
+        <v>1</v>
+      </c>
+      <c r="AT40" s="4">
+        <v>1</v>
+      </c>
       <c r="AU40" s="4"/>
-      <c r="AV40" s="4"/>
-      <c r="AW40" s="5"/>
+      <c r="AV40" s="4">
+        <v>1</v>
+      </c>
+      <c r="AW40" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="41" spans="1:49">
       <c r="A41" t="s">
@@ -5493,7 +5523,9 @@
       <c r="AL41" s="7">
         <v>1</v>
       </c>
-      <c r="AM41" s="7"/>
+      <c r="AM41" s="7">
+        <v>1</v>
+      </c>
       <c r="AN41" s="7"/>
       <c r="AO41" s="8"/>
       <c r="AP41" s="9"/>
@@ -5610,7 +5642,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F3E5D1B-61DD-7541-B70F-39B12913C18D}">
   <dimension ref="A1:AG40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="T16" sqref="T16"/>
     </sheetView>
   </sheetViews>
@@ -7555,13 +7587,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:AE40">
-    <cfRule type="cellIs" dxfId="0" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="27" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="1" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12108,54 +12140,54 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="W1:BJ40">
-    <cfRule type="cellIs" dxfId="90" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="9" operator="equal">
       <formula>9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="89" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="10" operator="equal">
       <formula>7</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="88" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="11" operator="equal">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="87" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="12" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="13" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="85" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="14" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="15" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="83" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="17" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y81:BL120">
-    <cfRule type="cellIs" dxfId="82" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="1" operator="equal">
       <formula>9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="2" operator="equal">
       <formula>7</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="3" operator="equal">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="79" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="4" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="5" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="77" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="6" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="7" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="8" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16294,54 +16326,54 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="W1:BJ40">
-    <cfRule type="cellIs" dxfId="74" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="9" operator="equal">
       <formula>9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="10" operator="equal">
       <formula>7</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="11" operator="equal">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="71" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="12" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="13" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="14" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="15" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="16" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y81:BL120">
-    <cfRule type="cellIs" dxfId="66" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="1" operator="equal">
       <formula>9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="2" operator="equal">
       <formula>7</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="3" operator="equal">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="4" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="5" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="6" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="7" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="8" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20542,184 +20574,184 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="AT16:AY17 AT15 AT18 AN20:AN21 W1:BJ1 AL4:AL6 W39:BJ40 W2:W38 AL12 AL21:AM21 AM2:BJ6 AX19:AY19 AX14:AY14 AW13:AY13 BA7:BJ24 AM22:AZ24 Y2:AK6 AG12:AK21 Y7:AE24 AF22:AK24 AO14:AR20 AM8:AN11 AT8:AZ8 AO9:AS13 AF8:AK10 AG11:AL11 AO21:AS21 AT20:AY21 AU9:AZ10 AT11:AY12 AM25:BJ25 BE26:BJ38 AB27:BD38 Y25:AK25 Y26:AA38 AM26:BD26 AB26:AK26">
-    <cfRule type="cellIs" dxfId="58" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="57" operator="equal">
       <formula>9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="58" operator="equal">
       <formula>7</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="59" operator="equal">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="60" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="61" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="62" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="63" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="64" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y81:BL120">
-    <cfRule type="cellIs" dxfId="50" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="49" operator="equal">
       <formula>9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="50" operator="equal">
       <formula>7</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="51" operator="equal">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="52" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="53" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="54" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="55" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="56" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU15:AX15">
-    <cfRule type="cellIs" dxfId="42" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="41" operator="equal">
       <formula>9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="42" operator="equal">
       <formula>7</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="43" operator="equal">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="44" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="45" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="46" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="47" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="48" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU18:AX18">
-    <cfRule type="cellIs" dxfId="34" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="33" operator="equal">
       <formula>9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="34" operator="equal">
       <formula>7</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="35" operator="equal">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="36" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="37" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="38" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="39" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="40" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AT19:AW19">
-    <cfRule type="cellIs" dxfId="26" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="25" operator="equal">
       <formula>9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="26" operator="equal">
       <formula>7</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="27" operator="equal">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="28" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="29" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="30" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="31" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="32" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AT14:AW14">
-    <cfRule type="cellIs" dxfId="18" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="9" operator="equal">
       <formula>9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="10" operator="equal">
       <formula>7</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="11" operator="equal">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="14" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="15" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="16" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AT13:AV13">
-    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>7</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="7" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="8" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
successfully implements first picture! :)
</commit_message>
<xml_diff>
--- a/prep/characters8bit.xlsx
+++ b/prep/characters8bit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tiago/Documents/github/my-patch-of-the-web/prep/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43A43F0D-5180-5249-97C2-9C18D7959D69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0494F9B5-7130-EE48-AF2F-1DA42B5AFDC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3840" yWindow="460" windowWidth="18960" windowHeight="13900" xr2:uid="{B2589E65-E8B1-364E-A64F-D98FD440D3EC}"/>
+    <workbookView xWindow="-31200" yWindow="2800" windowWidth="25620" windowHeight="15240" activeTab="1" xr2:uid="{B2589E65-E8B1-364E-A64F-D98FD440D3EC}"/>
   </bookViews>
   <sheets>
     <sheet name="letters" sheetId="1" r:id="rId1"/>
@@ -1193,7 +1193,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.89996032593768116"/>
+          <bgColor rgb="FFC00000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1207,7 +1207,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC00000"/>
+          <bgColor theme="2" tint="-0.89996032593768116"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1667,7 +1667,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{478EC196-EA3D-0B42-9BCE-C9EAFA77170C}">
   <dimension ref="A1:AW41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+    <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
       <selection activeCell="AV43" sqref="AV43"/>
     </sheetView>
   </sheetViews>
@@ -5640,18 +5640,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F3E5D1B-61DD-7541-B70F-39B12913C18D}">
-  <dimension ref="A1:AG40"/>
+  <dimension ref="A1:AQ40"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="T16" sqref="T16"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AF13" sqref="AF13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="2" max="31" width="3.83203125" style="10" customWidth="1"/>
+    <col min="2" max="41" width="3.83203125" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33">
+    <row r="1" spans="1:43">
       <c r="A1">
         <f>13*8*8</f>
         <v>832</v>
@@ -5685,17 +5685,25 @@
       <c r="AB1" s="12"/>
       <c r="AC1" s="12"/>
       <c r="AD1" s="12"/>
-      <c r="AE1" s="13"/>
-      <c r="AG1">
-        <f>SUM(B1:AE20)</f>
-        <v>347</v>
-      </c>
-    </row>
-    <row r="2" spans="1:33">
+      <c r="AE1" s="12"/>
+      <c r="AF1" s="12"/>
+      <c r="AG1" s="12"/>
+      <c r="AH1" s="12"/>
+      <c r="AI1" s="12"/>
+      <c r="AJ1" s="12"/>
+      <c r="AK1" s="12"/>
+      <c r="AL1" s="12"/>
+      <c r="AM1" s="12"/>
+      <c r="AN1" s="12"/>
+      <c r="AO1" s="13"/>
+      <c r="AQ1">
+        <f>SUM(B1:AO20)</f>
+        <v>564</v>
+      </c>
+    </row>
+    <row r="2" spans="1:43">
       <c r="B2" s="14"/>
-      <c r="C2" s="1">
-        <v>2</v>
-      </c>
+      <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -5723,136 +5731,174 @@
       <c r="AB2" s="1"/>
       <c r="AC2" s="1"/>
       <c r="AD2" s="1"/>
-      <c r="AE2" s="15"/>
-    </row>
-    <row r="3" spans="1:33">
+      <c r="AE2" s="1"/>
+      <c r="AF2" s="1"/>
+      <c r="AG2" s="1"/>
+      <c r="AH2" s="1"/>
+      <c r="AI2" s="1"/>
+      <c r="AJ2" s="1"/>
+      <c r="AK2" s="1"/>
+      <c r="AL2" s="1"/>
+      <c r="AM2" s="1"/>
+      <c r="AN2" s="1"/>
+      <c r="AO2" s="15"/>
+    </row>
+    <row r="3" spans="1:43">
       <c r="B3" s="14"/>
-      <c r="C3" s="1">
-        <v>2</v>
-      </c>
+      <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
-      <c r="I3" s="1">
-        <v>3</v>
-      </c>
-      <c r="Q3" s="1">
-        <v>3</v>
-      </c>
+      <c r="I3" s="1"/>
+      <c r="Q3" s="1"/>
       <c r="AB3" s="1"/>
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
-      <c r="AE3" s="15"/>
-    </row>
-    <row r="4" spans="1:33">
+      <c r="AE3" s="1"/>
+      <c r="AF3" s="1"/>
+      <c r="AG3" s="1"/>
+      <c r="AH3" s="1"/>
+      <c r="AI3" s="1"/>
+      <c r="AJ3" s="1"/>
+      <c r="AK3" s="1"/>
+      <c r="AL3" s="1"/>
+      <c r="AM3" s="1"/>
+      <c r="AN3" s="1"/>
+      <c r="AO3" s="15"/>
+    </row>
+    <row r="4" spans="1:43">
       <c r="B4" s="14"/>
-      <c r="C4" s="1">
-        <v>2</v>
-      </c>
+      <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="F4" s="1">
-        <v>3</v>
-      </c>
+      <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="1">
-        <v>3</v>
-      </c>
-      <c r="J4" s="1">
-        <v>3</v>
-      </c>
-      <c r="P4" s="1">
-        <v>3</v>
-      </c>
-      <c r="R4" s="1">
-        <v>3</v>
-      </c>
+      <c r="H4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="R4" s="1"/>
       <c r="AB4" s="1"/>
       <c r="AC4" s="1"/>
       <c r="AD4" s="1"/>
-      <c r="AE4" s="15"/>
-    </row>
-    <row r="5" spans="1:33">
+      <c r="AE4" s="1"/>
+      <c r="AF4" s="1"/>
+      <c r="AG4" s="1"/>
+      <c r="AH4" s="1"/>
+      <c r="AI4" s="1">
+        <v>6</v>
+      </c>
+      <c r="AJ4" s="1">
+        <v>6</v>
+      </c>
+      <c r="AK4" s="1">
+        <v>6</v>
+      </c>
+      <c r="AL4" s="1">
+        <v>6</v>
+      </c>
+      <c r="AM4" s="1"/>
+      <c r="AN4" s="1"/>
+      <c r="AO4" s="15"/>
+    </row>
+    <row r="5" spans="1:43">
       <c r="B5" s="14"/>
-      <c r="C5" s="1">
-        <v>2</v>
-      </c>
+      <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="1">
-        <v>3</v>
-      </c>
-      <c r="G5" s="1">
-        <v>3</v>
-      </c>
-      <c r="K5" s="1">
-        <v>3</v>
-      </c>
-      <c r="O5" s="1">
-        <v>3</v>
-      </c>
-      <c r="S5" s="1">
-        <v>3</v>
-      </c>
+      <c r="E5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="S5" s="1"/>
       <c r="AB5" s="1"/>
       <c r="AC5" s="1"/>
       <c r="AD5" s="1"/>
-      <c r="AE5" s="15"/>
-    </row>
-    <row r="6" spans="1:33">
+      <c r="AE5" s="1"/>
+      <c r="AF5" s="1"/>
+      <c r="AG5" s="1"/>
+      <c r="AH5" s="1"/>
+      <c r="AI5" s="1">
+        <v>6</v>
+      </c>
+      <c r="AJ5" s="1">
+        <v>6</v>
+      </c>
+      <c r="AK5" s="1">
+        <v>6</v>
+      </c>
+      <c r="AL5" s="1">
+        <v>6</v>
+      </c>
+      <c r="AM5" s="1"/>
+      <c r="AN5" s="1"/>
+      <c r="AO5" s="15"/>
+    </row>
+    <row r="6" spans="1:43">
       <c r="B6" s="14"/>
-      <c r="C6" s="1">
-        <v>2</v>
-      </c>
-      <c r="D6" s="1">
-        <v>3</v>
-      </c>
-      <c r="L6" s="1">
-        <v>3</v>
-      </c>
-      <c r="N6" s="1">
-        <v>3</v>
-      </c>
-      <c r="T6" s="1">
-        <v>3</v>
-      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="T6" s="1"/>
       <c r="AB6" s="1"/>
       <c r="AC6" s="1"/>
       <c r="AD6" s="1"/>
-      <c r="AE6" s="15"/>
-    </row>
-    <row r="7" spans="1:33">
+      <c r="AE6" s="1"/>
+      <c r="AF6" s="1"/>
+      <c r="AG6" s="1"/>
+      <c r="AH6" s="1"/>
+      <c r="AI6" s="1">
+        <v>6</v>
+      </c>
+      <c r="AJ6" s="1">
+        <v>6</v>
+      </c>
+      <c r="AK6" s="1">
+        <v>6</v>
+      </c>
+      <c r="AL6" s="1">
+        <v>6</v>
+      </c>
+      <c r="AM6" s="1"/>
+      <c r="AN6" s="1"/>
+      <c r="AO6" s="15"/>
+    </row>
+    <row r="7" spans="1:43">
       <c r="B7" s="14"/>
-      <c r="C7" s="1">
-        <v>2</v>
-      </c>
+      <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-      <c r="M7" s="1">
-        <v>3</v>
-      </c>
-      <c r="U7" s="1">
-        <v>3</v>
-      </c>
+      <c r="M7" s="1"/>
+      <c r="U7" s="1"/>
       <c r="AB7" s="1"/>
       <c r="AC7" s="1"/>
       <c r="AD7" s="1"/>
-      <c r="AE7" s="15"/>
-    </row>
-    <row r="8" spans="1:33">
+      <c r="AE7" s="1"/>
+      <c r="AF7" s="1"/>
+      <c r="AG7" s="1"/>
+      <c r="AH7" s="1"/>
+      <c r="AI7" s="1">
+        <v>6</v>
+      </c>
+      <c r="AJ7" s="1">
+        <v>6</v>
+      </c>
+      <c r="AK7" s="1">
+        <v>6</v>
+      </c>
+      <c r="AL7" s="1">
+        <v>6</v>
+      </c>
+      <c r="AM7" s="1"/>
+      <c r="AN7" s="1"/>
+      <c r="AO7" s="15"/>
+    </row>
+    <row r="8" spans="1:43">
       <c r="B8" s="14"/>
-      <c r="C8" s="1">
-        <v>2</v>
-      </c>
+      <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="1">
-        <v>1</v>
-      </c>
-      <c r="F8" s="1">
-        <v>1</v>
-      </c>
-      <c r="G8" s="1">
-        <v>1</v>
-      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -5867,9 +5913,7 @@
       <c r="S8" s="1"/>
       <c r="T8" s="1"/>
       <c r="U8" s="1"/>
-      <c r="V8" s="1">
-        <v>3</v>
-      </c>
+      <c r="V8" s="1"/>
       <c r="W8" s="1"/>
       <c r="X8" s="1"/>
       <c r="Y8" s="1"/>
@@ -5878,23 +5922,33 @@
       <c r="AB8" s="1"/>
       <c r="AC8" s="1"/>
       <c r="AD8" s="1"/>
-      <c r="AE8" s="15"/>
-    </row>
-    <row r="9" spans="1:33">
+      <c r="AE8" s="1"/>
+      <c r="AF8" s="1"/>
+      <c r="AG8" s="1"/>
+      <c r="AH8" s="1"/>
+      <c r="AI8" s="1">
+        <v>6</v>
+      </c>
+      <c r="AJ8" s="1">
+        <v>6</v>
+      </c>
+      <c r="AK8" s="1">
+        <v>6</v>
+      </c>
+      <c r="AL8" s="1">
+        <v>6</v>
+      </c>
+      <c r="AM8" s="1"/>
+      <c r="AN8" s="1"/>
+      <c r="AO8" s="15"/>
+    </row>
+    <row r="9" spans="1:43">
       <c r="B9" s="14"/>
-      <c r="C9" s="1">
-        <v>2</v>
-      </c>
+      <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="1">
-        <v>1</v>
-      </c>
-      <c r="F9" s="1">
-        <v>1</v>
-      </c>
-      <c r="G9" s="1">
-        <v>1</v>
-      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -5910,9 +5964,7 @@
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
       <c r="V9" s="1"/>
-      <c r="W9" s="1">
-        <v>3</v>
-      </c>
+      <c r="W9" s="1"/>
       <c r="X9" s="1"/>
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
@@ -5920,13 +5972,29 @@
       <c r="AB9" s="1"/>
       <c r="AC9" s="1"/>
       <c r="AD9" s="1"/>
-      <c r="AE9" s="15"/>
-    </row>
-    <row r="10" spans="1:33">
+      <c r="AE9" s="1"/>
+      <c r="AF9" s="1"/>
+      <c r="AG9" s="1"/>
+      <c r="AH9" s="1"/>
+      <c r="AI9" s="1">
+        <v>6</v>
+      </c>
+      <c r="AJ9" s="1">
+        <v>6</v>
+      </c>
+      <c r="AK9" s="1">
+        <v>6</v>
+      </c>
+      <c r="AL9" s="1">
+        <v>6</v>
+      </c>
+      <c r="AM9" s="1"/>
+      <c r="AN9" s="1"/>
+      <c r="AO9" s="15"/>
+    </row>
+    <row r="10" spans="1:43">
       <c r="B10" s="14"/>
-      <c r="C10" s="1">
-        <v>2</v>
-      </c>
+      <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1">
         <v>1</v>
@@ -5937,7 +6005,9 @@
       <c r="G10" s="1">
         <v>1</v>
       </c>
-      <c r="H10" s="1"/>
+      <c r="H10" s="1">
+        <v>1</v>
+      </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
@@ -5953,22 +6023,36 @@
       <c r="U10" s="1"/>
       <c r="V10" s="1"/>
       <c r="W10" s="1"/>
-      <c r="X10" s="1">
-        <v>3</v>
-      </c>
+      <c r="X10" s="1"/>
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
       <c r="AA10" s="1"/>
       <c r="AB10" s="1"/>
       <c r="AC10" s="1"/>
       <c r="AD10" s="1"/>
-      <c r="AE10" s="15"/>
-    </row>
-    <row r="11" spans="1:33">
+      <c r="AE10" s="1"/>
+      <c r="AF10" s="1"/>
+      <c r="AG10" s="1"/>
+      <c r="AH10" s="1"/>
+      <c r="AI10" s="1">
+        <v>6</v>
+      </c>
+      <c r="AJ10" s="1">
+        <v>6</v>
+      </c>
+      <c r="AK10" s="1">
+        <v>6</v>
+      </c>
+      <c r="AL10" s="1">
+        <v>6</v>
+      </c>
+      <c r="AM10" s="1"/>
+      <c r="AN10" s="1"/>
+      <c r="AO10" s="15"/>
+    </row>
+    <row r="11" spans="1:43">
       <c r="B11" s="14"/>
-      <c r="C11" s="1">
-        <v>2</v>
-      </c>
+      <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1">
         <v>1</v>
@@ -5979,16 +6063,15 @@
       <c r="G11" s="1">
         <v>1</v>
       </c>
-      <c r="H11" s="1"/>
+      <c r="H11" s="1">
+        <v>1</v>
+      </c>
       <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
@@ -5996,21 +6079,35 @@
       <c r="V11" s="1"/>
       <c r="W11" s="1"/>
       <c r="X11" s="1"/>
-      <c r="Y11" s="1">
-        <v>3</v>
-      </c>
+      <c r="Y11" s="1"/>
       <c r="Z11" s="1"/>
       <c r="AA11" s="1"/>
       <c r="AB11" s="1"/>
       <c r="AC11" s="1"/>
       <c r="AD11" s="1"/>
-      <c r="AE11" s="15"/>
-    </row>
-    <row r="12" spans="1:33">
+      <c r="AE11" s="1"/>
+      <c r="AF11" s="1"/>
+      <c r="AG11" s="1"/>
+      <c r="AH11" s="1"/>
+      <c r="AI11" s="1">
+        <v>6</v>
+      </c>
+      <c r="AJ11" s="1">
+        <v>6</v>
+      </c>
+      <c r="AK11" s="1">
+        <v>6</v>
+      </c>
+      <c r="AL11" s="1">
+        <v>6</v>
+      </c>
+      <c r="AM11" s="1"/>
+      <c r="AN11" s="1"/>
+      <c r="AO11" s="15"/>
+    </row>
+    <row r="12" spans="1:43">
       <c r="B12" s="14"/>
-      <c r="C12" s="1">
-        <v>2</v>
-      </c>
+      <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1">
         <v>1</v>
@@ -6021,22 +6118,16 @@
       <c r="G12" s="1">
         <v>1</v>
       </c>
-      <c r="H12" s="1"/>
+      <c r="H12" s="1">
+        <v>1</v>
+      </c>
       <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
-      <c r="O12" s="1">
-        <v>5</v>
-      </c>
-      <c r="P12" s="1">
-        <v>5</v>
-      </c>
-      <c r="Q12" s="1">
-        <v>5</v>
-      </c>
+      <c r="O12" s="1"/>
+      <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
       <c r="T12" s="1"/>
@@ -6045,20 +6136,33 @@
       <c r="W12" s="1"/>
       <c r="X12" s="1"/>
       <c r="Y12" s="1"/>
-      <c r="Z12" s="1">
-        <v>3</v>
-      </c>
+      <c r="Z12" s="1"/>
       <c r="AA12" s="1"/>
       <c r="AB12" s="1"/>
       <c r="AC12" s="1"/>
-      <c r="AD12" s="1"/>
-      <c r="AE12" s="15"/>
-    </row>
-    <row r="13" spans="1:33">
+      <c r="AE12" s="1"/>
+      <c r="AF12" s="1"/>
+      <c r="AG12" s="1"/>
+      <c r="AH12" s="1"/>
+      <c r="AI12" s="1">
+        <v>6</v>
+      </c>
+      <c r="AJ12" s="1">
+        <v>6</v>
+      </c>
+      <c r="AK12" s="1">
+        <v>6</v>
+      </c>
+      <c r="AL12" s="1">
+        <v>6</v>
+      </c>
+      <c r="AM12" s="1"/>
+      <c r="AN12" s="1"/>
+      <c r="AO12" s="15"/>
+    </row>
+    <row r="13" spans="1:43">
       <c r="B13" s="14"/>
-      <c r="C13" s="1">
-        <v>2</v>
-      </c>
+      <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1">
         <v>1</v>
@@ -6069,22 +6173,16 @@
       <c r="G13" s="1">
         <v>1</v>
       </c>
-      <c r="H13" s="1"/>
+      <c r="H13" s="1">
+        <v>1</v>
+      </c>
       <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
-      <c r="O13" s="1">
-        <v>5</v>
-      </c>
-      <c r="P13" s="1">
-        <v>5</v>
-      </c>
-      <c r="Q13" s="1">
-        <v>5</v>
-      </c>
+      <c r="O13" s="1"/>
+      <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
       <c r="T13" s="1"/>
@@ -6094,19 +6192,32 @@
       <c r="X13" s="1"/>
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
-      <c r="AA13" s="1">
-        <v>3</v>
-      </c>
+      <c r="AA13" s="1"/>
       <c r="AB13" s="1"/>
       <c r="AC13" s="1"/>
-      <c r="AD13" s="1"/>
-      <c r="AE13" s="15"/>
-    </row>
-    <row r="14" spans="1:33">
+      <c r="AE13" s="1"/>
+      <c r="AF13" s="1"/>
+      <c r="AG13" s="1"/>
+      <c r="AH13" s="1"/>
+      <c r="AI13" s="1">
+        <v>6</v>
+      </c>
+      <c r="AJ13" s="1">
+        <v>6</v>
+      </c>
+      <c r="AK13" s="1">
+        <v>6</v>
+      </c>
+      <c r="AL13" s="1">
+        <v>6</v>
+      </c>
+      <c r="AM13" s="1"/>
+      <c r="AN13" s="1"/>
+      <c r="AO13" s="15"/>
+    </row>
+    <row r="14" spans="1:43">
       <c r="B14" s="14"/>
-      <c r="C14" s="1">
-        <v>2</v>
-      </c>
+      <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1">
         <v>1</v>
@@ -6117,25 +6228,27 @@
       <c r="G14" s="1">
         <v>1</v>
       </c>
-      <c r="H14" s="1"/>
+      <c r="H14" s="1">
+        <v>1</v>
+      </c>
       <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
-      <c r="O14" s="1">
-        <v>5</v>
-      </c>
-      <c r="P14" s="1">
-        <v>5</v>
-      </c>
+      <c r="O14" s="1"/>
       <c r="Q14" s="1">
-        <v>5</v>
-      </c>
-      <c r="R14" s="1"/>
-      <c r="S14" s="1"/>
-      <c r="T14" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="R14" s="1">
+        <v>3</v>
+      </c>
+      <c r="S14" s="1">
+        <v>3</v>
+      </c>
+      <c r="T14" s="1">
+        <v>3</v>
+      </c>
       <c r="U14" s="1"/>
       <c r="V14" s="1"/>
       <c r="W14" s="1"/>
@@ -6143,18 +6256,31 @@
       <c r="Y14" s="1"/>
       <c r="Z14" s="1"/>
       <c r="AA14" s="1"/>
-      <c r="AB14" s="1">
-        <v>3</v>
-      </c>
+      <c r="AB14" s="1"/>
       <c r="AC14" s="1"/>
-      <c r="AD14" s="1"/>
-      <c r="AE14" s="15"/>
-    </row>
-    <row r="15" spans="1:33">
+      <c r="AE14" s="1"/>
+      <c r="AF14" s="1"/>
+      <c r="AG14" s="1"/>
+      <c r="AH14" s="1"/>
+      <c r="AI14" s="1">
+        <v>6</v>
+      </c>
+      <c r="AJ14" s="1">
+        <v>6</v>
+      </c>
+      <c r="AK14" s="1">
+        <v>6</v>
+      </c>
+      <c r="AL14" s="1">
+        <v>6</v>
+      </c>
+      <c r="AM14" s="1"/>
+      <c r="AN14" s="1"/>
+      <c r="AO14" s="15"/>
+    </row>
+    <row r="15" spans="1:43">
       <c r="B15" s="14"/>
-      <c r="C15" s="1">
-        <v>2</v>
-      </c>
+      <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1">
         <v>1</v>
@@ -6165,25 +6291,27 @@
       <c r="G15" s="1">
         <v>1</v>
       </c>
-      <c r="H15" s="1"/>
+      <c r="H15" s="1">
+        <v>1</v>
+      </c>
       <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
-      <c r="O15" s="1">
-        <v>5</v>
-      </c>
-      <c r="P15" s="1">
-        <v>5</v>
-      </c>
+      <c r="O15" s="1"/>
       <c r="Q15" s="1">
-        <v>5</v>
-      </c>
-      <c r="R15" s="1"/>
-      <c r="S15" s="1"/>
-      <c r="T15" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="R15" s="1">
+        <v>3</v>
+      </c>
+      <c r="S15" s="1">
+        <v>3</v>
+      </c>
+      <c r="T15" s="1">
+        <v>3</v>
+      </c>
       <c r="U15" s="1"/>
       <c r="V15" s="1"/>
       <c r="W15" s="1"/>
@@ -6192,17 +6320,30 @@
       <c r="Z15" s="1"/>
       <c r="AA15" s="1"/>
       <c r="AB15" s="1"/>
-      <c r="AC15" s="1">
-        <v>3</v>
-      </c>
-      <c r="AD15" s="1"/>
-      <c r="AE15" s="15"/>
-    </row>
-    <row r="16" spans="1:33">
+      <c r="AC15" s="1"/>
+      <c r="AE15" s="1"/>
+      <c r="AF15" s="1"/>
+      <c r="AG15" s="1"/>
+      <c r="AH15" s="1"/>
+      <c r="AI15" s="1">
+        <v>6</v>
+      </c>
+      <c r="AJ15" s="1">
+        <v>6</v>
+      </c>
+      <c r="AK15" s="1">
+        <v>6</v>
+      </c>
+      <c r="AL15" s="1">
+        <v>6</v>
+      </c>
+      <c r="AM15" s="1"/>
+      <c r="AN15" s="1"/>
+      <c r="AO15" s="15"/>
+    </row>
+    <row r="16" spans="1:43">
       <c r="B16" s="14"/>
-      <c r="C16" s="1">
-        <v>2</v>
-      </c>
+      <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1">
         <v>1</v>
@@ -6213,25 +6354,27 @@
       <c r="G16" s="1">
         <v>1</v>
       </c>
-      <c r="H16" s="1"/>
+      <c r="H16" s="1">
+        <v>1</v>
+      </c>
       <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
-      <c r="O16" s="1">
-        <v>5</v>
-      </c>
-      <c r="P16" s="1">
-        <v>5</v>
-      </c>
+      <c r="O16" s="1"/>
       <c r="Q16" s="1">
-        <v>5</v>
-      </c>
-      <c r="R16" s="1"/>
-      <c r="S16" s="1"/>
-      <c r="T16" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="R16" s="1">
+        <v>3</v>
+      </c>
+      <c r="S16" s="1">
+        <v>3</v>
+      </c>
+      <c r="T16" s="1">
+        <v>3</v>
+      </c>
       <c r="U16" s="1"/>
       <c r="V16" s="1"/>
       <c r="W16" s="1"/>
@@ -6241,14 +6384,29 @@
       <c r="AA16" s="1"/>
       <c r="AB16" s="1"/>
       <c r="AC16" s="1"/>
-      <c r="AD16" s="1"/>
-      <c r="AE16" s="15"/>
-    </row>
-    <row r="17" spans="2:31">
+      <c r="AE16" s="1"/>
+      <c r="AF16" s="1"/>
+      <c r="AG16" s="1"/>
+      <c r="AH16" s="1"/>
+      <c r="AI16" s="1">
+        <v>6</v>
+      </c>
+      <c r="AJ16" s="1">
+        <v>6</v>
+      </c>
+      <c r="AK16" s="1">
+        <v>6</v>
+      </c>
+      <c r="AL16" s="1">
+        <v>6</v>
+      </c>
+      <c r="AM16" s="1"/>
+      <c r="AN16" s="1"/>
+      <c r="AO16" s="15"/>
+    </row>
+    <row r="17" spans="2:41">
       <c r="B17" s="14"/>
-      <c r="C17" s="1">
-        <v>2</v>
-      </c>
+      <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1">
         <v>1</v>
@@ -6259,25 +6417,27 @@
       <c r="G17" s="1">
         <v>1</v>
       </c>
-      <c r="H17" s="1"/>
+      <c r="H17" s="1">
+        <v>1</v>
+      </c>
       <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
-      <c r="O17" s="1">
-        <v>5</v>
-      </c>
-      <c r="P17" s="1">
-        <v>5</v>
-      </c>
+      <c r="O17" s="1"/>
       <c r="Q17" s="1">
-        <v>5</v>
-      </c>
-      <c r="R17" s="1"/>
-      <c r="S17" s="1"/>
-      <c r="T17" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="R17" s="1">
+        <v>3</v>
+      </c>
+      <c r="S17" s="1">
+        <v>3</v>
+      </c>
+      <c r="T17" s="1">
+        <v>3</v>
+      </c>
       <c r="U17" s="1"/>
       <c r="V17" s="1"/>
       <c r="W17" s="1"/>
@@ -6287,14 +6447,29 @@
       <c r="AA17" s="1"/>
       <c r="AB17" s="1"/>
       <c r="AC17" s="1"/>
-      <c r="AD17" s="1"/>
-      <c r="AE17" s="15"/>
-    </row>
-    <row r="18" spans="2:31">
+      <c r="AE17" s="1"/>
+      <c r="AF17" s="1"/>
+      <c r="AG17" s="1"/>
+      <c r="AH17" s="1"/>
+      <c r="AI17" s="1">
+        <v>6</v>
+      </c>
+      <c r="AJ17" s="1">
+        <v>6</v>
+      </c>
+      <c r="AK17" s="1">
+        <v>6</v>
+      </c>
+      <c r="AL17" s="1">
+        <v>6</v>
+      </c>
+      <c r="AM17" s="1"/>
+      <c r="AN17" s="1"/>
+      <c r="AO17" s="15"/>
+    </row>
+    <row r="18" spans="2:41">
       <c r="B18" s="14"/>
-      <c r="C18" s="1">
-        <v>2</v>
-      </c>
+      <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1">
         <v>1</v>
@@ -6305,31 +6480,27 @@
       <c r="G18" s="1">
         <v>1</v>
       </c>
-      <c r="H18" s="1"/>
+      <c r="H18" s="1">
+        <v>1</v>
+      </c>
       <c r="I18" s="1"/>
-      <c r="J18" s="1">
-        <v>4</v>
-      </c>
-      <c r="K18" s="1">
-        <v>4</v>
-      </c>
-      <c r="L18" s="1">
-        <v>4</v>
-      </c>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
-      <c r="O18" s="1">
-        <v>5</v>
-      </c>
-      <c r="P18" s="1">
-        <v>5</v>
-      </c>
+      <c r="O18" s="1"/>
       <c r="Q18" s="1">
-        <v>5</v>
-      </c>
-      <c r="R18" s="1"/>
-      <c r="S18" s="1"/>
-      <c r="T18" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="R18" s="1">
+        <v>3</v>
+      </c>
+      <c r="S18" s="1">
+        <v>3</v>
+      </c>
+      <c r="T18" s="1">
+        <v>3</v>
+      </c>
       <c r="U18" s="1"/>
       <c r="V18" s="1"/>
       <c r="W18" s="1"/>
@@ -6339,14 +6510,29 @@
       <c r="AA18" s="1"/>
       <c r="AB18" s="1"/>
       <c r="AC18" s="1"/>
-      <c r="AD18" s="1"/>
-      <c r="AE18" s="15"/>
-    </row>
-    <row r="19" spans="2:31">
+      <c r="AE18" s="1"/>
+      <c r="AF18" s="1"/>
+      <c r="AG18" s="1"/>
+      <c r="AH18" s="1"/>
+      <c r="AI18" s="1">
+        <v>6</v>
+      </c>
+      <c r="AJ18" s="1">
+        <v>6</v>
+      </c>
+      <c r="AK18" s="1">
+        <v>6</v>
+      </c>
+      <c r="AL18" s="1">
+        <v>6</v>
+      </c>
+      <c r="AM18" s="1"/>
+      <c r="AN18" s="1"/>
+      <c r="AO18" s="15"/>
+    </row>
+    <row r="19" spans="2:41">
       <c r="B19" s="14"/>
-      <c r="C19" s="1">
-        <v>2</v>
-      </c>
+      <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1">
         <v>1</v>
@@ -6357,31 +6543,27 @@
       <c r="G19" s="1">
         <v>1</v>
       </c>
-      <c r="H19" s="1"/>
+      <c r="H19" s="1">
+        <v>1</v>
+      </c>
       <c r="I19" s="1"/>
-      <c r="J19" s="1">
-        <v>4</v>
-      </c>
-      <c r="K19" s="1">
-        <v>4</v>
-      </c>
-      <c r="L19" s="1">
-        <v>4</v>
-      </c>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
-      <c r="O19" s="1">
-        <v>5</v>
-      </c>
-      <c r="P19" s="1">
-        <v>5</v>
-      </c>
+      <c r="O19" s="1"/>
       <c r="Q19" s="1">
-        <v>5</v>
-      </c>
-      <c r="R19" s="1"/>
-      <c r="S19" s="1"/>
-      <c r="T19" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="R19" s="1">
+        <v>3</v>
+      </c>
+      <c r="S19" s="1">
+        <v>3</v>
+      </c>
+      <c r="T19" s="1">
+        <v>3</v>
+      </c>
       <c r="U19" s="1"/>
       <c r="V19" s="1"/>
       <c r="W19" s="1"/>
@@ -6391,14 +6573,29 @@
       <c r="AA19" s="1"/>
       <c r="AB19" s="1"/>
       <c r="AC19" s="1"/>
-      <c r="AD19" s="1"/>
-      <c r="AE19" s="15"/>
-    </row>
-    <row r="20" spans="2:31">
+      <c r="AE19" s="1"/>
+      <c r="AF19" s="1"/>
+      <c r="AG19" s="1"/>
+      <c r="AH19" s="1"/>
+      <c r="AI19" s="1">
+        <v>6</v>
+      </c>
+      <c r="AJ19" s="1">
+        <v>6</v>
+      </c>
+      <c r="AK19" s="1">
+        <v>6</v>
+      </c>
+      <c r="AL19" s="1">
+        <v>6</v>
+      </c>
+      <c r="AM19" s="1"/>
+      <c r="AN19" s="1"/>
+      <c r="AO19" s="15"/>
+    </row>
+    <row r="20" spans="2:41">
       <c r="B20" s="14"/>
-      <c r="C20" s="1">
-        <v>2</v>
-      </c>
+      <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1">
         <v>1</v>
@@ -6409,54 +6606,74 @@
       <c r="G20" s="1">
         <v>1</v>
       </c>
-      <c r="H20" s="1"/>
+      <c r="H20" s="1">
+        <v>1</v>
+      </c>
       <c r="I20" s="1"/>
-      <c r="J20" s="1">
-        <v>4</v>
-      </c>
       <c r="K20" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L20" s="1">
-        <v>4</v>
-      </c>
-      <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
-      <c r="O20" s="1">
-        <v>5</v>
-      </c>
-      <c r="P20" s="1">
-        <v>5</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="M20" s="1">
+        <v>2</v>
+      </c>
+      <c r="N20" s="1">
+        <v>2</v>
+      </c>
+      <c r="O20" s="1"/>
       <c r="Q20" s="1">
-        <v>5</v>
-      </c>
-      <c r="R20" s="1"/>
-      <c r="S20" s="1"/>
-      <c r="T20" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="R20" s="1">
+        <v>3</v>
+      </c>
+      <c r="S20" s="1">
+        <v>3</v>
+      </c>
+      <c r="T20" s="1">
+        <v>3</v>
+      </c>
       <c r="U20" s="1"/>
-      <c r="V20" s="1"/>
       <c r="W20" s="1"/>
       <c r="X20" s="1"/>
-      <c r="Y20" s="1">
-        <v>7</v>
-      </c>
-      <c r="Z20" s="1">
-        <v>7</v>
-      </c>
-      <c r="AA20" s="1">
-        <v>7</v>
-      </c>
-      <c r="AB20" s="1"/>
-      <c r="AC20" s="1"/>
-      <c r="AD20" s="1"/>
-      <c r="AE20" s="15"/>
-    </row>
-    <row r="21" spans="2:31">
+      <c r="Y20" s="1"/>
+      <c r="Z20" s="1"/>
+      <c r="AA20" s="1"/>
+      <c r="AC20" s="1">
+        <v>5</v>
+      </c>
+      <c r="AD20" s="1">
+        <v>5</v>
+      </c>
+      <c r="AE20" s="1">
+        <v>5</v>
+      </c>
+      <c r="AF20" s="1">
+        <v>5</v>
+      </c>
+      <c r="AG20" s="1"/>
+      <c r="AH20" s="1"/>
+      <c r="AI20" s="1">
+        <v>6</v>
+      </c>
+      <c r="AJ20" s="1">
+        <v>6</v>
+      </c>
+      <c r="AK20" s="1">
+        <v>6</v>
+      </c>
+      <c r="AL20" s="1">
+        <v>6</v>
+      </c>
+      <c r="AM20" s="1"/>
+      <c r="AN20" s="1"/>
+      <c r="AO20" s="15"/>
+    </row>
+    <row r="21" spans="2:41">
       <c r="B21" s="14"/>
-      <c r="C21" s="1">
-        <v>2</v>
-      </c>
+      <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1">
         <v>1</v>
@@ -6467,54 +6684,74 @@
       <c r="G21" s="1">
         <v>1</v>
       </c>
-      <c r="H21" s="1"/>
+      <c r="H21" s="1">
+        <v>1</v>
+      </c>
       <c r="I21" s="1"/>
-      <c r="J21" s="1">
-        <v>4</v>
-      </c>
       <c r="K21" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L21" s="1">
-        <v>4</v>
-      </c>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
-      <c r="O21" s="1">
-        <v>5</v>
-      </c>
-      <c r="P21" s="1">
-        <v>5</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="M21" s="1">
+        <v>2</v>
+      </c>
+      <c r="N21" s="1">
+        <v>2</v>
+      </c>
+      <c r="O21" s="1"/>
       <c r="Q21" s="1">
-        <v>5</v>
-      </c>
-      <c r="R21" s="1"/>
-      <c r="S21" s="1"/>
-      <c r="T21" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="R21" s="1">
+        <v>3</v>
+      </c>
+      <c r="S21" s="1">
+        <v>3</v>
+      </c>
+      <c r="T21" s="1">
+        <v>3</v>
+      </c>
       <c r="U21" s="1"/>
-      <c r="V21" s="1"/>
       <c r="W21" s="1"/>
       <c r="X21" s="1"/>
-      <c r="Y21" s="1">
-        <v>7</v>
-      </c>
-      <c r="Z21" s="1">
-        <v>7</v>
-      </c>
-      <c r="AA21" s="1">
-        <v>7</v>
-      </c>
-      <c r="AB21" s="1"/>
-      <c r="AC21" s="1"/>
-      <c r="AD21" s="1"/>
-      <c r="AE21" s="15"/>
-    </row>
-    <row r="22" spans="2:31">
+      <c r="Y21" s="1"/>
+      <c r="Z21" s="1"/>
+      <c r="AA21" s="1"/>
+      <c r="AC21" s="1">
+        <v>5</v>
+      </c>
+      <c r="AD21" s="1">
+        <v>5</v>
+      </c>
+      <c r="AE21" s="1">
+        <v>5</v>
+      </c>
+      <c r="AF21" s="1">
+        <v>5</v>
+      </c>
+      <c r="AG21" s="1"/>
+      <c r="AH21" s="1"/>
+      <c r="AI21" s="1">
+        <v>6</v>
+      </c>
+      <c r="AJ21" s="1">
+        <v>6</v>
+      </c>
+      <c r="AK21" s="1">
+        <v>6</v>
+      </c>
+      <c r="AL21" s="1">
+        <v>6</v>
+      </c>
+      <c r="AM21" s="1"/>
+      <c r="AN21" s="1"/>
+      <c r="AO21" s="15"/>
+    </row>
+    <row r="22" spans="2:41">
       <c r="B22" s="14"/>
-      <c r="C22" s="1">
-        <v>2</v>
-      </c>
+      <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1">
         <v>1</v>
@@ -6525,54 +6762,74 @@
       <c r="G22" s="1">
         <v>1</v>
       </c>
-      <c r="H22" s="1"/>
+      <c r="H22" s="1">
+        <v>1</v>
+      </c>
       <c r="I22" s="1"/>
-      <c r="J22" s="1">
-        <v>4</v>
-      </c>
       <c r="K22" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L22" s="1">
-        <v>4</v>
-      </c>
-      <c r="M22" s="1"/>
-      <c r="N22" s="1"/>
-      <c r="O22" s="1">
-        <v>5</v>
-      </c>
-      <c r="P22" s="1">
-        <v>5</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="M22" s="1">
+        <v>2</v>
+      </c>
+      <c r="N22" s="1">
+        <v>2</v>
+      </c>
+      <c r="O22" s="1"/>
       <c r="Q22" s="1">
-        <v>5</v>
-      </c>
-      <c r="R22" s="1"/>
-      <c r="S22" s="1"/>
-      <c r="T22" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="R22" s="1">
+        <v>3</v>
+      </c>
+      <c r="S22" s="1">
+        <v>3</v>
+      </c>
+      <c r="T22" s="1">
+        <v>3</v>
+      </c>
       <c r="U22" s="1"/>
-      <c r="V22" s="1"/>
       <c r="W22" s="1"/>
       <c r="X22" s="1"/>
-      <c r="Y22" s="1">
-        <v>7</v>
-      </c>
-      <c r="Z22" s="1">
-        <v>7</v>
-      </c>
-      <c r="AA22" s="1">
-        <v>7</v>
-      </c>
-      <c r="AB22" s="1"/>
-      <c r="AC22" s="1"/>
-      <c r="AD22" s="1"/>
-      <c r="AE22" s="15"/>
-    </row>
-    <row r="23" spans="2:31">
+      <c r="Y22" s="1"/>
+      <c r="Z22" s="1"/>
+      <c r="AA22" s="1"/>
+      <c r="AC22" s="1">
+        <v>5</v>
+      </c>
+      <c r="AD22" s="1">
+        <v>5</v>
+      </c>
+      <c r="AE22" s="1">
+        <v>5</v>
+      </c>
+      <c r="AF22" s="1">
+        <v>5</v>
+      </c>
+      <c r="AG22" s="1"/>
+      <c r="AH22" s="1"/>
+      <c r="AI22" s="1">
+        <v>6</v>
+      </c>
+      <c r="AJ22" s="1">
+        <v>6</v>
+      </c>
+      <c r="AK22" s="1">
+        <v>6</v>
+      </c>
+      <c r="AL22" s="1">
+        <v>6</v>
+      </c>
+      <c r="AM22" s="1"/>
+      <c r="AN22" s="1"/>
+      <c r="AO22" s="15"/>
+    </row>
+    <row r="23" spans="2:41">
       <c r="B23" s="14"/>
-      <c r="C23" s="1">
-        <v>2</v>
-      </c>
+      <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1">
         <v>1</v>
@@ -6583,54 +6840,74 @@
       <c r="G23" s="1">
         <v>1</v>
       </c>
-      <c r="H23" s="1"/>
+      <c r="H23" s="1">
+        <v>1</v>
+      </c>
       <c r="I23" s="1"/>
-      <c r="J23" s="1">
-        <v>4</v>
-      </c>
       <c r="K23" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L23" s="1">
-        <v>4</v>
-      </c>
-      <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
-      <c r="O23" s="1">
-        <v>5</v>
-      </c>
-      <c r="P23" s="1">
-        <v>5</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="M23" s="1">
+        <v>2</v>
+      </c>
+      <c r="N23" s="1">
+        <v>2</v>
+      </c>
+      <c r="O23" s="1"/>
       <c r="Q23" s="1">
-        <v>5</v>
-      </c>
-      <c r="R23" s="1"/>
-      <c r="S23" s="1"/>
-      <c r="T23" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="R23" s="1">
+        <v>3</v>
+      </c>
+      <c r="S23" s="1">
+        <v>3</v>
+      </c>
+      <c r="T23" s="1">
+        <v>3</v>
+      </c>
       <c r="U23" s="1"/>
-      <c r="V23" s="1"/>
       <c r="W23" s="1"/>
       <c r="X23" s="1"/>
-      <c r="Y23" s="1">
-        <v>7</v>
-      </c>
-      <c r="Z23" s="1">
-        <v>7</v>
-      </c>
-      <c r="AA23" s="1">
-        <v>7</v>
-      </c>
-      <c r="AB23" s="1"/>
-      <c r="AC23" s="1"/>
-      <c r="AD23" s="1"/>
-      <c r="AE23" s="15"/>
-    </row>
-    <row r="24" spans="2:31">
+      <c r="Y23" s="1"/>
+      <c r="Z23" s="1"/>
+      <c r="AA23" s="1"/>
+      <c r="AC23" s="1">
+        <v>5</v>
+      </c>
+      <c r="AD23" s="1">
+        <v>5</v>
+      </c>
+      <c r="AE23" s="1">
+        <v>5</v>
+      </c>
+      <c r="AF23" s="1">
+        <v>5</v>
+      </c>
+      <c r="AG23" s="1"/>
+      <c r="AH23" s="1"/>
+      <c r="AI23" s="1">
+        <v>6</v>
+      </c>
+      <c r="AJ23" s="1">
+        <v>6</v>
+      </c>
+      <c r="AK23" s="1">
+        <v>6</v>
+      </c>
+      <c r="AL23" s="1">
+        <v>6</v>
+      </c>
+      <c r="AM23" s="1"/>
+      <c r="AN23" s="1"/>
+      <c r="AO23" s="15"/>
+    </row>
+    <row r="24" spans="2:41">
       <c r="B24" s="14"/>
-      <c r="C24" s="1">
-        <v>2</v>
-      </c>
+      <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1">
         <v>1</v>
@@ -6641,54 +6918,74 @@
       <c r="G24" s="1">
         <v>1</v>
       </c>
-      <c r="H24" s="1"/>
+      <c r="H24" s="1">
+        <v>1</v>
+      </c>
       <c r="I24" s="1"/>
-      <c r="J24" s="1">
-        <v>4</v>
-      </c>
       <c r="K24" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L24" s="1">
-        <v>4</v>
-      </c>
-      <c r="M24" s="1"/>
-      <c r="N24" s="1"/>
-      <c r="O24" s="1">
-        <v>5</v>
-      </c>
-      <c r="P24" s="1">
-        <v>5</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="M24" s="1">
+        <v>2</v>
+      </c>
+      <c r="N24" s="1">
+        <v>2</v>
+      </c>
+      <c r="O24" s="1"/>
       <c r="Q24" s="1">
-        <v>5</v>
-      </c>
-      <c r="R24" s="1"/>
-      <c r="S24" s="1"/>
-      <c r="T24" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="R24" s="1">
+        <v>3</v>
+      </c>
+      <c r="S24" s="1">
+        <v>3</v>
+      </c>
+      <c r="T24" s="1">
+        <v>3</v>
+      </c>
       <c r="U24" s="1"/>
-      <c r="V24" s="1"/>
       <c r="W24" s="1"/>
       <c r="X24" s="1"/>
-      <c r="Y24" s="1">
-        <v>7</v>
-      </c>
-      <c r="Z24" s="1">
-        <v>7</v>
-      </c>
-      <c r="AA24" s="1">
-        <v>7</v>
-      </c>
-      <c r="AB24" s="1"/>
-      <c r="AC24" s="1"/>
-      <c r="AD24" s="1"/>
-      <c r="AE24" s="15"/>
-    </row>
-    <row r="25" spans="2:31">
+      <c r="Y24" s="1"/>
+      <c r="Z24" s="1"/>
+      <c r="AA24" s="1"/>
+      <c r="AC24" s="1">
+        <v>5</v>
+      </c>
+      <c r="AD24" s="1">
+        <v>5</v>
+      </c>
+      <c r="AE24" s="1">
+        <v>5</v>
+      </c>
+      <c r="AF24" s="1">
+        <v>5</v>
+      </c>
+      <c r="AG24" s="1"/>
+      <c r="AH24" s="1"/>
+      <c r="AI24" s="1">
+        <v>6</v>
+      </c>
+      <c r="AJ24" s="1">
+        <v>6</v>
+      </c>
+      <c r="AK24" s="1">
+        <v>6</v>
+      </c>
+      <c r="AL24" s="1">
+        <v>6</v>
+      </c>
+      <c r="AM24" s="1"/>
+      <c r="AN24" s="1"/>
+      <c r="AO24" s="15"/>
+    </row>
+    <row r="25" spans="2:41">
       <c r="B25" s="14"/>
-      <c r="C25" s="1">
-        <v>2</v>
-      </c>
+      <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1">
         <v>1</v>
@@ -6699,60 +6996,82 @@
       <c r="G25" s="1">
         <v>1</v>
       </c>
-      <c r="H25" s="1"/>
+      <c r="H25" s="1">
+        <v>1</v>
+      </c>
       <c r="I25" s="1"/>
-      <c r="J25" s="1">
+      <c r="K25" s="1">
+        <v>2</v>
+      </c>
+      <c r="L25" s="1">
+        <v>2</v>
+      </c>
+      <c r="M25" s="1">
+        <v>2</v>
+      </c>
+      <c r="N25" s="1">
+        <v>2</v>
+      </c>
+      <c r="O25" s="1"/>
+      <c r="Q25" s="1">
+        <v>3</v>
+      </c>
+      <c r="R25" s="1">
+        <v>3</v>
+      </c>
+      <c r="S25" s="1">
+        <v>3</v>
+      </c>
+      <c r="T25" s="1">
+        <v>3</v>
+      </c>
+      <c r="U25" s="1"/>
+      <c r="W25" s="1">
         <v>4</v>
       </c>
-      <c r="K25" s="1">
+      <c r="X25" s="1">
         <v>4</v>
       </c>
-      <c r="L25" s="1">
+      <c r="Y25" s="1">
         <v>4</v>
       </c>
-      <c r="M25" s="1"/>
-      <c r="N25" s="1"/>
-      <c r="O25" s="1">
+      <c r="Z25" s="1">
+        <v>4</v>
+      </c>
+      <c r="AA25" s="1"/>
+      <c r="AC25" s="1">
         <v>5</v>
       </c>
-      <c r="P25" s="1">
+      <c r="AD25" s="1">
         <v>5</v>
       </c>
-      <c r="Q25" s="1">
+      <c r="AE25" s="1">
         <v>5</v>
       </c>
-      <c r="R25" s="1"/>
-      <c r="S25" s="1"/>
-      <c r="T25" s="1">
+      <c r="AF25" s="1">
+        <v>5</v>
+      </c>
+      <c r="AG25" s="1"/>
+      <c r="AH25" s="1"/>
+      <c r="AI25" s="1">
         <v>6</v>
       </c>
-      <c r="U25" s="1">
+      <c r="AJ25" s="1">
         <v>6</v>
       </c>
-      <c r="V25" s="1">
+      <c r="AK25" s="1">
         <v>6</v>
       </c>
-      <c r="W25" s="1"/>
-      <c r="X25" s="1"/>
-      <c r="Y25" s="1">
-        <v>7</v>
-      </c>
-      <c r="Z25" s="1">
-        <v>7</v>
-      </c>
-      <c r="AA25" s="1">
-        <v>7</v>
-      </c>
-      <c r="AB25" s="1"/>
-      <c r="AC25" s="1"/>
-      <c r="AD25" s="1"/>
-      <c r="AE25" s="15"/>
-    </row>
-    <row r="26" spans="2:31">
+      <c r="AL25" s="1">
+        <v>6</v>
+      </c>
+      <c r="AM25" s="1"/>
+      <c r="AN25" s="1"/>
+      <c r="AO25" s="15"/>
+    </row>
+    <row r="26" spans="2:41">
       <c r="B26" s="14"/>
-      <c r="C26" s="1">
-        <v>2</v>
-      </c>
+      <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1">
         <v>1</v>
@@ -6763,60 +7082,82 @@
       <c r="G26" s="1">
         <v>1</v>
       </c>
-      <c r="H26" s="1"/>
+      <c r="H26" s="1">
+        <v>1</v>
+      </c>
       <c r="I26" s="1"/>
-      <c r="J26" s="1">
+      <c r="K26" s="1">
+        <v>2</v>
+      </c>
+      <c r="L26" s="1">
+        <v>2</v>
+      </c>
+      <c r="M26" s="1">
+        <v>2</v>
+      </c>
+      <c r="N26" s="1">
+        <v>2</v>
+      </c>
+      <c r="O26" s="1"/>
+      <c r="Q26" s="1">
+        <v>3</v>
+      </c>
+      <c r="R26" s="1">
+        <v>3</v>
+      </c>
+      <c r="S26" s="1">
+        <v>3</v>
+      </c>
+      <c r="T26" s="1">
+        <v>3</v>
+      </c>
+      <c r="U26" s="1"/>
+      <c r="W26" s="1">
         <v>4</v>
       </c>
-      <c r="K26" s="1">
+      <c r="X26" s="1">
         <v>4</v>
       </c>
-      <c r="L26" s="1">
+      <c r="Y26" s="1">
         <v>4</v>
       </c>
-      <c r="M26" s="1"/>
-      <c r="N26" s="1"/>
-      <c r="O26" s="1">
+      <c r="Z26" s="1">
+        <v>4</v>
+      </c>
+      <c r="AA26" s="1"/>
+      <c r="AC26" s="1">
         <v>5</v>
       </c>
-      <c r="P26" s="1">
+      <c r="AD26" s="1">
         <v>5</v>
       </c>
-      <c r="Q26" s="1">
+      <c r="AE26" s="1">
         <v>5</v>
       </c>
-      <c r="R26" s="1"/>
-      <c r="S26" s="1"/>
-      <c r="T26" s="1">
+      <c r="AF26" s="1">
+        <v>5</v>
+      </c>
+      <c r="AG26" s="1"/>
+      <c r="AH26" s="1"/>
+      <c r="AI26" s="1">
         <v>6</v>
       </c>
-      <c r="U26" s="1">
+      <c r="AJ26" s="1">
         <v>6</v>
       </c>
-      <c r="V26" s="1">
+      <c r="AK26" s="1">
         <v>6</v>
       </c>
-      <c r="W26" s="1"/>
-      <c r="X26" s="1"/>
-      <c r="Y26" s="1">
-        <v>7</v>
-      </c>
-      <c r="Z26" s="1">
-        <v>7</v>
-      </c>
-      <c r="AA26" s="1">
-        <v>7</v>
-      </c>
-      <c r="AB26" s="1"/>
-      <c r="AC26" s="1"/>
-      <c r="AD26" s="1"/>
-      <c r="AE26" s="15"/>
-    </row>
-    <row r="27" spans="2:31">
+      <c r="AL26" s="1">
+        <v>6</v>
+      </c>
+      <c r="AM26" s="1"/>
+      <c r="AN26" s="1"/>
+      <c r="AO26" s="15"/>
+    </row>
+    <row r="27" spans="2:41">
       <c r="B27" s="14"/>
-      <c r="C27" s="1">
-        <v>2</v>
-      </c>
+      <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1">
         <v>1</v>
@@ -6827,60 +7168,82 @@
       <c r="G27" s="1">
         <v>1</v>
       </c>
-      <c r="H27" s="1"/>
+      <c r="H27" s="1">
+        <v>1</v>
+      </c>
       <c r="I27" s="1"/>
-      <c r="J27" s="1">
+      <c r="K27" s="1">
+        <v>2</v>
+      </c>
+      <c r="L27" s="1">
+        <v>2</v>
+      </c>
+      <c r="M27" s="1">
+        <v>2</v>
+      </c>
+      <c r="N27" s="1">
+        <v>2</v>
+      </c>
+      <c r="O27" s="1"/>
+      <c r="Q27" s="1">
+        <v>3</v>
+      </c>
+      <c r="R27" s="1">
+        <v>3</v>
+      </c>
+      <c r="S27" s="1">
+        <v>3</v>
+      </c>
+      <c r="T27" s="1">
+        <v>3</v>
+      </c>
+      <c r="U27" s="1"/>
+      <c r="W27" s="1">
         <v>4</v>
       </c>
-      <c r="K27" s="1">
+      <c r="X27" s="1">
         <v>4</v>
       </c>
-      <c r="L27" s="1">
+      <c r="Y27" s="1">
         <v>4</v>
       </c>
-      <c r="M27" s="1"/>
-      <c r="N27" s="1"/>
-      <c r="O27" s="1">
+      <c r="Z27" s="1">
+        <v>4</v>
+      </c>
+      <c r="AA27" s="1"/>
+      <c r="AC27" s="1">
         <v>5</v>
       </c>
-      <c r="P27" s="1">
+      <c r="AD27" s="1">
         <v>5</v>
       </c>
-      <c r="Q27" s="1">
+      <c r="AE27" s="1">
         <v>5</v>
       </c>
-      <c r="R27" s="1"/>
-      <c r="S27" s="1"/>
-      <c r="T27" s="1">
+      <c r="AF27" s="1">
+        <v>5</v>
+      </c>
+      <c r="AG27" s="1"/>
+      <c r="AH27" s="1"/>
+      <c r="AI27" s="1">
         <v>6</v>
       </c>
-      <c r="U27" s="1">
+      <c r="AJ27" s="1">
         <v>6</v>
       </c>
-      <c r="V27" s="1">
+      <c r="AK27" s="1">
         <v>6</v>
       </c>
-      <c r="W27" s="1"/>
-      <c r="X27" s="1"/>
-      <c r="Y27" s="1">
-        <v>7</v>
-      </c>
-      <c r="Z27" s="1">
-        <v>7</v>
-      </c>
-      <c r="AA27" s="1">
-        <v>7</v>
-      </c>
-      <c r="AB27" s="1"/>
-      <c r="AC27" s="1"/>
-      <c r="AD27" s="1"/>
-      <c r="AE27" s="15"/>
-    </row>
-    <row r="28" spans="2:31">
+      <c r="AL27" s="1">
+        <v>6</v>
+      </c>
+      <c r="AM27" s="1"/>
+      <c r="AN27" s="1"/>
+      <c r="AO27" s="15"/>
+    </row>
+    <row r="28" spans="2:41">
       <c r="B28" s="14"/>
-      <c r="C28" s="1">
-        <v>2</v>
-      </c>
+      <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1">
         <v>1</v>
@@ -6891,60 +7254,82 @@
       <c r="G28" s="1">
         <v>1</v>
       </c>
-      <c r="H28" s="1"/>
+      <c r="H28" s="1">
+        <v>1</v>
+      </c>
       <c r="I28" s="1"/>
-      <c r="J28" s="1">
+      <c r="K28" s="1">
+        <v>2</v>
+      </c>
+      <c r="L28" s="1">
+        <v>2</v>
+      </c>
+      <c r="M28" s="1">
+        <v>2</v>
+      </c>
+      <c r="N28" s="1">
+        <v>2</v>
+      </c>
+      <c r="O28" s="1"/>
+      <c r="Q28" s="1">
+        <v>3</v>
+      </c>
+      <c r="R28" s="1">
+        <v>3</v>
+      </c>
+      <c r="S28" s="1">
+        <v>3</v>
+      </c>
+      <c r="T28" s="1">
+        <v>3</v>
+      </c>
+      <c r="U28" s="1"/>
+      <c r="W28" s="1">
         <v>4</v>
       </c>
-      <c r="K28" s="1">
+      <c r="X28" s="1">
         <v>4</v>
       </c>
-      <c r="L28" s="1">
+      <c r="Y28" s="1">
         <v>4</v>
       </c>
-      <c r="M28" s="1"/>
-      <c r="N28" s="1"/>
-      <c r="O28" s="1">
+      <c r="Z28" s="1">
+        <v>4</v>
+      </c>
+      <c r="AA28" s="1"/>
+      <c r="AC28" s="1">
         <v>5</v>
       </c>
-      <c r="P28" s="1">
+      <c r="AD28" s="1">
         <v>5</v>
       </c>
-      <c r="Q28" s="1">
+      <c r="AE28" s="1">
         <v>5</v>
       </c>
-      <c r="R28" s="1"/>
-      <c r="S28" s="1"/>
-      <c r="T28" s="1">
+      <c r="AF28" s="1">
+        <v>5</v>
+      </c>
+      <c r="AG28" s="1"/>
+      <c r="AH28" s="1"/>
+      <c r="AI28" s="1">
         <v>6</v>
       </c>
-      <c r="U28" s="1">
+      <c r="AJ28" s="1">
         <v>6</v>
       </c>
-      <c r="V28" s="1">
+      <c r="AK28" s="1">
         <v>6</v>
       </c>
-      <c r="W28" s="1"/>
-      <c r="X28" s="1"/>
-      <c r="Y28" s="1">
-        <v>7</v>
-      </c>
-      <c r="Z28" s="1">
-        <v>7</v>
-      </c>
-      <c r="AA28" s="1">
-        <v>7</v>
-      </c>
-      <c r="AB28" s="1"/>
-      <c r="AC28" s="1"/>
-      <c r="AD28" s="1"/>
-      <c r="AE28" s="15"/>
-    </row>
-    <row r="29" spans="2:31">
+      <c r="AL28" s="1">
+        <v>6</v>
+      </c>
+      <c r="AM28" s="1"/>
+      <c r="AN28" s="1"/>
+      <c r="AO28" s="15"/>
+    </row>
+    <row r="29" spans="2:41">
       <c r="B29" s="14"/>
-      <c r="C29" s="1">
-        <v>2</v>
-      </c>
+      <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1">
         <v>1</v>
@@ -6955,60 +7340,82 @@
       <c r="G29" s="1">
         <v>1</v>
       </c>
-      <c r="H29" s="1"/>
+      <c r="H29" s="1">
+        <v>1</v>
+      </c>
       <c r="I29" s="1"/>
-      <c r="J29" s="1">
+      <c r="K29" s="1">
+        <v>2</v>
+      </c>
+      <c r="L29" s="1">
+        <v>2</v>
+      </c>
+      <c r="M29" s="1">
+        <v>2</v>
+      </c>
+      <c r="N29" s="1">
+        <v>2</v>
+      </c>
+      <c r="O29" s="1"/>
+      <c r="Q29" s="1">
+        <v>3</v>
+      </c>
+      <c r="R29" s="1">
+        <v>3</v>
+      </c>
+      <c r="S29" s="1">
+        <v>3</v>
+      </c>
+      <c r="T29" s="1">
+        <v>3</v>
+      </c>
+      <c r="U29" s="1"/>
+      <c r="W29" s="1">
         <v>4</v>
       </c>
-      <c r="K29" s="1">
+      <c r="X29" s="1">
         <v>4</v>
       </c>
-      <c r="L29" s="1">
+      <c r="Y29" s="1">
         <v>4</v>
       </c>
-      <c r="M29" s="1"/>
-      <c r="N29" s="1"/>
-      <c r="O29" s="1">
+      <c r="Z29" s="1">
+        <v>4</v>
+      </c>
+      <c r="AA29" s="1"/>
+      <c r="AC29" s="1">
         <v>5</v>
       </c>
-      <c r="P29" s="1">
+      <c r="AD29" s="1">
         <v>5</v>
       </c>
-      <c r="Q29" s="1">
+      <c r="AE29" s="1">
         <v>5</v>
       </c>
-      <c r="R29" s="1"/>
-      <c r="S29" s="1"/>
-      <c r="T29" s="1">
+      <c r="AF29" s="1">
+        <v>5</v>
+      </c>
+      <c r="AG29" s="1"/>
+      <c r="AH29" s="1"/>
+      <c r="AI29" s="1">
         <v>6</v>
       </c>
-      <c r="U29" s="1">
+      <c r="AJ29" s="1">
         <v>6</v>
       </c>
-      <c r="V29" s="1">
+      <c r="AK29" s="1">
         <v>6</v>
       </c>
-      <c r="W29" s="1"/>
-      <c r="X29" s="1"/>
-      <c r="Y29" s="1">
-        <v>7</v>
-      </c>
-      <c r="Z29" s="1">
-        <v>7</v>
-      </c>
-      <c r="AA29" s="1">
-        <v>7</v>
-      </c>
-      <c r="AB29" s="1"/>
-      <c r="AC29" s="1"/>
-      <c r="AD29" s="1"/>
-      <c r="AE29" s="15"/>
-    </row>
-    <row r="30" spans="2:31">
+      <c r="AL29" s="1">
+        <v>6</v>
+      </c>
+      <c r="AM29" s="1"/>
+      <c r="AN29" s="1"/>
+      <c r="AO29" s="15"/>
+    </row>
+    <row r="30" spans="2:41">
       <c r="B30" s="14"/>
-      <c r="C30" s="1">
-        <v>2</v>
-      </c>
+      <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1">
         <v>1</v>
@@ -7019,60 +7426,82 @@
       <c r="G30" s="1">
         <v>1</v>
       </c>
-      <c r="H30" s="1"/>
+      <c r="H30" s="1">
+        <v>1</v>
+      </c>
       <c r="I30" s="1"/>
-      <c r="J30" s="1">
+      <c r="K30" s="1">
+        <v>2</v>
+      </c>
+      <c r="L30" s="1">
+        <v>2</v>
+      </c>
+      <c r="M30" s="1">
+        <v>2</v>
+      </c>
+      <c r="N30" s="1">
+        <v>2</v>
+      </c>
+      <c r="O30" s="1"/>
+      <c r="Q30" s="1">
+        <v>3</v>
+      </c>
+      <c r="R30" s="1">
+        <v>3</v>
+      </c>
+      <c r="S30" s="1">
+        <v>3</v>
+      </c>
+      <c r="T30" s="1">
+        <v>3</v>
+      </c>
+      <c r="U30" s="1"/>
+      <c r="W30" s="1">
         <v>4</v>
       </c>
-      <c r="K30" s="1">
+      <c r="X30" s="1">
         <v>4</v>
       </c>
-      <c r="L30" s="1">
+      <c r="Y30" s="1">
         <v>4</v>
       </c>
-      <c r="M30" s="1"/>
-      <c r="N30" s="1"/>
-      <c r="O30" s="1">
+      <c r="Z30" s="1">
+        <v>4</v>
+      </c>
+      <c r="AA30" s="1"/>
+      <c r="AC30" s="1">
         <v>5</v>
       </c>
-      <c r="P30" s="1">
+      <c r="AD30" s="1">
         <v>5</v>
       </c>
-      <c r="Q30" s="1">
+      <c r="AE30" s="1">
         <v>5</v>
       </c>
-      <c r="R30" s="1"/>
-      <c r="S30" s="1"/>
-      <c r="T30" s="1">
+      <c r="AF30" s="1">
+        <v>5</v>
+      </c>
+      <c r="AG30" s="1"/>
+      <c r="AH30" s="1"/>
+      <c r="AI30" s="1">
         <v>6</v>
       </c>
-      <c r="U30" s="1">
+      <c r="AJ30" s="1">
         <v>6</v>
       </c>
-      <c r="V30" s="1">
+      <c r="AK30" s="1">
         <v>6</v>
       </c>
-      <c r="W30" s="1"/>
-      <c r="X30" s="1"/>
-      <c r="Y30" s="1">
-        <v>7</v>
-      </c>
-      <c r="Z30" s="1">
-        <v>7</v>
-      </c>
-      <c r="AA30" s="1">
-        <v>7</v>
-      </c>
-      <c r="AB30" s="1"/>
-      <c r="AC30" s="1"/>
-      <c r="AD30" s="1"/>
-      <c r="AE30" s="15"/>
-    </row>
-    <row r="31" spans="2:31">
+      <c r="AL30" s="1">
+        <v>6</v>
+      </c>
+      <c r="AM30" s="1"/>
+      <c r="AN30" s="1"/>
+      <c r="AO30" s="15"/>
+    </row>
+    <row r="31" spans="2:41">
       <c r="B31" s="14"/>
-      <c r="C31" s="1">
-        <v>2</v>
-      </c>
+      <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1">
         <v>1</v>
@@ -7083,60 +7512,82 @@
       <c r="G31" s="1">
         <v>1</v>
       </c>
-      <c r="H31" s="1"/>
+      <c r="H31" s="1">
+        <v>1</v>
+      </c>
       <c r="I31" s="1"/>
-      <c r="J31" s="1">
+      <c r="K31" s="1">
+        <v>2</v>
+      </c>
+      <c r="L31" s="1">
+        <v>2</v>
+      </c>
+      <c r="M31" s="1">
+        <v>2</v>
+      </c>
+      <c r="N31" s="1">
+        <v>2</v>
+      </c>
+      <c r="O31" s="1"/>
+      <c r="Q31" s="1">
+        <v>3</v>
+      </c>
+      <c r="R31" s="1">
+        <v>3</v>
+      </c>
+      <c r="S31" s="1">
+        <v>3</v>
+      </c>
+      <c r="T31" s="1">
+        <v>3</v>
+      </c>
+      <c r="U31" s="1"/>
+      <c r="W31" s="1">
         <v>4</v>
       </c>
-      <c r="K31" s="1">
+      <c r="X31" s="1">
         <v>4</v>
       </c>
-      <c r="L31" s="1">
+      <c r="Y31" s="1">
         <v>4</v>
       </c>
-      <c r="M31" s="1"/>
-      <c r="N31" s="1"/>
-      <c r="O31" s="1">
+      <c r="Z31" s="1">
+        <v>4</v>
+      </c>
+      <c r="AA31" s="1"/>
+      <c r="AC31" s="1">
         <v>5</v>
       </c>
-      <c r="P31" s="1">
+      <c r="AD31" s="1">
         <v>5</v>
       </c>
-      <c r="Q31" s="1">
+      <c r="AE31" s="1">
         <v>5</v>
       </c>
-      <c r="R31" s="1"/>
-      <c r="S31" s="1"/>
-      <c r="T31" s="1">
+      <c r="AF31" s="1">
+        <v>5</v>
+      </c>
+      <c r="AG31" s="1"/>
+      <c r="AH31" s="1"/>
+      <c r="AI31" s="1">
         <v>6</v>
       </c>
-      <c r="U31" s="1">
+      <c r="AJ31" s="1">
         <v>6</v>
       </c>
-      <c r="V31" s="1">
+      <c r="AK31" s="1">
         <v>6</v>
       </c>
-      <c r="W31" s="1"/>
-      <c r="X31" s="1"/>
-      <c r="Y31" s="1">
-        <v>7</v>
-      </c>
-      <c r="Z31" s="1">
-        <v>7</v>
-      </c>
-      <c r="AA31" s="1">
-        <v>7</v>
-      </c>
-      <c r="AB31" s="1"/>
-      <c r="AC31" s="1"/>
-      <c r="AD31" s="1"/>
-      <c r="AE31" s="15"/>
-    </row>
-    <row r="32" spans="2:31">
+      <c r="AL31" s="1">
+        <v>6</v>
+      </c>
+      <c r="AM31" s="1"/>
+      <c r="AN31" s="1"/>
+      <c r="AO31" s="15"/>
+    </row>
+    <row r="32" spans="2:41">
       <c r="B32" s="14"/>
-      <c r="C32" s="1">
-        <v>2</v>
-      </c>
+      <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1">
         <v>1</v>
@@ -7147,60 +7598,82 @@
       <c r="G32" s="1">
         <v>1</v>
       </c>
-      <c r="H32" s="1"/>
+      <c r="H32" s="1">
+        <v>1</v>
+      </c>
       <c r="I32" s="1"/>
-      <c r="J32" s="1">
+      <c r="K32" s="1">
+        <v>2</v>
+      </c>
+      <c r="L32" s="1">
+        <v>2</v>
+      </c>
+      <c r="M32" s="1">
+        <v>2</v>
+      </c>
+      <c r="N32" s="1">
+        <v>2</v>
+      </c>
+      <c r="O32" s="1"/>
+      <c r="Q32" s="1">
+        <v>3</v>
+      </c>
+      <c r="R32" s="1">
+        <v>3</v>
+      </c>
+      <c r="S32" s="1">
+        <v>3</v>
+      </c>
+      <c r="T32" s="1">
+        <v>3</v>
+      </c>
+      <c r="U32" s="1"/>
+      <c r="W32" s="1">
         <v>4</v>
       </c>
-      <c r="K32" s="1">
+      <c r="X32" s="1">
         <v>4</v>
       </c>
-      <c r="L32" s="1">
+      <c r="Y32" s="1">
         <v>4</v>
       </c>
-      <c r="M32" s="1"/>
-      <c r="N32" s="1"/>
-      <c r="O32" s="1">
+      <c r="Z32" s="1">
+        <v>4</v>
+      </c>
+      <c r="AA32" s="1"/>
+      <c r="AC32" s="1">
         <v>5</v>
       </c>
-      <c r="P32" s="1">
+      <c r="AD32" s="1">
         <v>5</v>
       </c>
-      <c r="Q32" s="1">
+      <c r="AE32" s="1">
         <v>5</v>
       </c>
-      <c r="R32" s="1"/>
-      <c r="S32" s="1"/>
-      <c r="T32" s="1">
+      <c r="AF32" s="1">
+        <v>5</v>
+      </c>
+      <c r="AG32" s="1"/>
+      <c r="AH32" s="1"/>
+      <c r="AI32" s="1">
         <v>6</v>
       </c>
-      <c r="U32" s="1">
+      <c r="AJ32" s="1">
         <v>6</v>
       </c>
-      <c r="V32" s="1">
+      <c r="AK32" s="1">
         <v>6</v>
       </c>
-      <c r="W32" s="1"/>
-      <c r="X32" s="1"/>
-      <c r="Y32" s="1">
-        <v>7</v>
-      </c>
-      <c r="Z32" s="1">
-        <v>7</v>
-      </c>
-      <c r="AA32" s="1">
-        <v>7</v>
-      </c>
-      <c r="AB32" s="1"/>
-      <c r="AC32" s="1"/>
-      <c r="AD32" s="1"/>
-      <c r="AE32" s="15"/>
-    </row>
-    <row r="33" spans="2:31">
+      <c r="AL32" s="1">
+        <v>6</v>
+      </c>
+      <c r="AM32" s="1"/>
+      <c r="AN32" s="1"/>
+      <c r="AO32" s="15"/>
+    </row>
+    <row r="33" spans="2:41">
       <c r="B33" s="14"/>
-      <c r="C33" s="1">
-        <v>2</v>
-      </c>
+      <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1">
         <v>1</v>
@@ -7211,60 +7684,82 @@
       <c r="G33" s="1">
         <v>1</v>
       </c>
-      <c r="H33" s="1"/>
+      <c r="H33" s="1">
+        <v>1</v>
+      </c>
       <c r="I33" s="1"/>
-      <c r="J33" s="1">
+      <c r="K33" s="1">
+        <v>2</v>
+      </c>
+      <c r="L33" s="1">
+        <v>2</v>
+      </c>
+      <c r="M33" s="1">
+        <v>2</v>
+      </c>
+      <c r="N33" s="1">
+        <v>2</v>
+      </c>
+      <c r="O33" s="1"/>
+      <c r="Q33" s="1">
+        <v>3</v>
+      </c>
+      <c r="R33" s="1">
+        <v>3</v>
+      </c>
+      <c r="S33" s="1">
+        <v>3</v>
+      </c>
+      <c r="T33" s="1">
+        <v>3</v>
+      </c>
+      <c r="U33" s="1"/>
+      <c r="W33" s="1">
         <v>4</v>
       </c>
-      <c r="K33" s="1">
+      <c r="X33" s="1">
         <v>4</v>
       </c>
-      <c r="L33" s="1">
+      <c r="Y33" s="1">
         <v>4</v>
       </c>
-      <c r="M33" s="1"/>
-      <c r="N33" s="1"/>
-      <c r="O33" s="1">
+      <c r="Z33" s="1">
+        <v>4</v>
+      </c>
+      <c r="AA33" s="1"/>
+      <c r="AC33" s="1">
         <v>5</v>
       </c>
-      <c r="P33" s="1">
+      <c r="AD33" s="1">
         <v>5</v>
       </c>
-      <c r="Q33" s="1">
+      <c r="AE33" s="1">
         <v>5</v>
       </c>
-      <c r="R33" s="1"/>
-      <c r="S33" s="1"/>
-      <c r="T33" s="1">
+      <c r="AF33" s="1">
+        <v>5</v>
+      </c>
+      <c r="AG33" s="1"/>
+      <c r="AH33" s="1"/>
+      <c r="AI33" s="1">
         <v>6</v>
       </c>
-      <c r="U33" s="1">
+      <c r="AJ33" s="1">
         <v>6</v>
       </c>
-      <c r="V33" s="1">
+      <c r="AK33" s="1">
         <v>6</v>
       </c>
-      <c r="W33" s="1"/>
-      <c r="X33" s="1"/>
-      <c r="Y33" s="1">
-        <v>7</v>
-      </c>
-      <c r="Z33" s="1">
-        <v>7</v>
-      </c>
-      <c r="AA33" s="1">
-        <v>7</v>
-      </c>
-      <c r="AB33" s="1"/>
-      <c r="AC33" s="1"/>
-      <c r="AD33" s="1"/>
-      <c r="AE33" s="15"/>
-    </row>
-    <row r="34" spans="2:31">
+      <c r="AL33" s="1">
+        <v>6</v>
+      </c>
+      <c r="AM33" s="1"/>
+      <c r="AN33" s="1"/>
+      <c r="AO33" s="15"/>
+    </row>
+    <row r="34" spans="2:41">
       <c r="B34" s="14"/>
-      <c r="C34" s="1">
-        <v>2</v>
-      </c>
+      <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1">
         <v>1</v>
@@ -7275,60 +7770,82 @@
       <c r="G34" s="1">
         <v>1</v>
       </c>
-      <c r="H34" s="1"/>
+      <c r="H34" s="1">
+        <v>1</v>
+      </c>
       <c r="I34" s="1"/>
-      <c r="J34" s="1">
+      <c r="K34" s="1">
+        <v>2</v>
+      </c>
+      <c r="L34" s="1">
+        <v>2</v>
+      </c>
+      <c r="M34" s="1">
+        <v>2</v>
+      </c>
+      <c r="N34" s="1">
+        <v>2</v>
+      </c>
+      <c r="O34" s="1"/>
+      <c r="Q34" s="1">
+        <v>3</v>
+      </c>
+      <c r="R34" s="1">
+        <v>3</v>
+      </c>
+      <c r="S34" s="1">
+        <v>3</v>
+      </c>
+      <c r="T34" s="1">
+        <v>3</v>
+      </c>
+      <c r="U34" s="1"/>
+      <c r="W34" s="1">
         <v>4</v>
       </c>
-      <c r="K34" s="1">
+      <c r="X34" s="1">
         <v>4</v>
       </c>
-      <c r="L34" s="1">
+      <c r="Y34" s="1">
         <v>4</v>
       </c>
-      <c r="M34" s="1"/>
-      <c r="N34" s="1"/>
-      <c r="O34" s="1">
+      <c r="Z34" s="1">
+        <v>4</v>
+      </c>
+      <c r="AA34" s="1"/>
+      <c r="AC34" s="1">
         <v>5</v>
       </c>
-      <c r="P34" s="1">
+      <c r="AD34" s="1">
         <v>5</v>
       </c>
-      <c r="Q34" s="1">
+      <c r="AE34" s="1">
         <v>5</v>
       </c>
-      <c r="R34" s="1"/>
-      <c r="S34" s="1"/>
-      <c r="T34" s="1">
+      <c r="AF34" s="1">
+        <v>5</v>
+      </c>
+      <c r="AG34" s="1"/>
+      <c r="AH34" s="1"/>
+      <c r="AI34" s="1">
         <v>6</v>
       </c>
-      <c r="U34" s="1">
+      <c r="AJ34" s="1">
         <v>6</v>
       </c>
-      <c r="V34" s="1">
+      <c r="AK34" s="1">
         <v>6</v>
       </c>
-      <c r="W34" s="1"/>
-      <c r="X34" s="1"/>
-      <c r="Y34" s="1">
-        <v>7</v>
-      </c>
-      <c r="Z34" s="1">
-        <v>7</v>
-      </c>
-      <c r="AA34" s="1">
-        <v>7</v>
-      </c>
-      <c r="AB34" s="1"/>
-      <c r="AC34" s="1"/>
-      <c r="AD34" s="1"/>
-      <c r="AE34" s="15"/>
-    </row>
-    <row r="35" spans="2:31">
+      <c r="AL34" s="1">
+        <v>6</v>
+      </c>
+      <c r="AM34" s="1"/>
+      <c r="AN34" s="1"/>
+      <c r="AO34" s="15"/>
+    </row>
+    <row r="35" spans="2:41">
       <c r="B35" s="14"/>
-      <c r="C35" s="1">
-        <v>2</v>
-      </c>
+      <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1">
         <v>1</v>
@@ -7339,60 +7856,82 @@
       <c r="G35" s="1">
         <v>1</v>
       </c>
-      <c r="H35" s="1"/>
+      <c r="H35" s="1">
+        <v>1</v>
+      </c>
       <c r="I35" s="1"/>
-      <c r="J35" s="1">
+      <c r="K35" s="1">
+        <v>2</v>
+      </c>
+      <c r="L35" s="1">
+        <v>2</v>
+      </c>
+      <c r="M35" s="1">
+        <v>2</v>
+      </c>
+      <c r="N35" s="1">
+        <v>2</v>
+      </c>
+      <c r="O35" s="1"/>
+      <c r="Q35" s="1">
+        <v>3</v>
+      </c>
+      <c r="R35" s="1">
+        <v>3</v>
+      </c>
+      <c r="S35" s="1">
+        <v>3</v>
+      </c>
+      <c r="T35" s="1">
+        <v>3</v>
+      </c>
+      <c r="U35" s="1"/>
+      <c r="W35" s="1">
         <v>4</v>
       </c>
-      <c r="K35" s="1">
+      <c r="X35" s="1">
         <v>4</v>
       </c>
-      <c r="L35" s="1">
+      <c r="Y35" s="1">
         <v>4</v>
       </c>
-      <c r="M35" s="1"/>
-      <c r="N35" s="1"/>
-      <c r="O35" s="1">
+      <c r="Z35" s="1">
+        <v>4</v>
+      </c>
+      <c r="AA35" s="1"/>
+      <c r="AC35" s="1">
         <v>5</v>
       </c>
-      <c r="P35" s="1">
+      <c r="AD35" s="1">
         <v>5</v>
       </c>
-      <c r="Q35" s="1">
+      <c r="AE35" s="1">
         <v>5</v>
       </c>
-      <c r="R35" s="1"/>
-      <c r="S35" s="1"/>
-      <c r="T35" s="1">
+      <c r="AF35" s="1">
+        <v>5</v>
+      </c>
+      <c r="AG35" s="1"/>
+      <c r="AH35" s="1"/>
+      <c r="AI35" s="1">
         <v>6</v>
       </c>
-      <c r="U35" s="1">
+      <c r="AJ35" s="1">
         <v>6</v>
       </c>
-      <c r="V35" s="1">
+      <c r="AK35" s="1">
         <v>6</v>
       </c>
-      <c r="W35" s="1"/>
-      <c r="X35" s="1"/>
-      <c r="Y35" s="1">
-        <v>7</v>
-      </c>
-      <c r="Z35" s="1">
-        <v>7</v>
-      </c>
-      <c r="AA35" s="1">
-        <v>7</v>
-      </c>
-      <c r="AB35" s="1"/>
-      <c r="AC35" s="1"/>
-      <c r="AD35" s="1"/>
-      <c r="AE35" s="15"/>
-    </row>
-    <row r="36" spans="2:31">
+      <c r="AL35" s="1">
+        <v>6</v>
+      </c>
+      <c r="AM35" s="1"/>
+      <c r="AN35" s="1"/>
+      <c r="AO35" s="15"/>
+    </row>
+    <row r="36" spans="2:41">
       <c r="B36" s="14"/>
-      <c r="C36" s="1">
-        <v>2</v>
-      </c>
+      <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1">
         <v>1</v>
@@ -7403,157 +7942,153 @@
       <c r="G36" s="1">
         <v>1</v>
       </c>
-      <c r="H36" s="1"/>
+      <c r="H36" s="1">
+        <v>1</v>
+      </c>
       <c r="I36" s="1"/>
-      <c r="J36" s="1">
+      <c r="K36" s="1">
+        <v>2</v>
+      </c>
+      <c r="L36" s="1">
+        <v>2</v>
+      </c>
+      <c r="M36" s="1">
+        <v>2</v>
+      </c>
+      <c r="N36" s="1">
+        <v>2</v>
+      </c>
+      <c r="O36" s="1"/>
+      <c r="Q36" s="1">
+        <v>3</v>
+      </c>
+      <c r="R36" s="1">
+        <v>3</v>
+      </c>
+      <c r="S36" s="1">
+        <v>3</v>
+      </c>
+      <c r="T36" s="1">
+        <v>3</v>
+      </c>
+      <c r="U36" s="1"/>
+      <c r="W36" s="1">
         <v>4</v>
       </c>
-      <c r="K36" s="1">
+      <c r="X36" s="1">
         <v>4</v>
       </c>
-      <c r="L36" s="1">
+      <c r="Y36" s="1">
         <v>4</v>
       </c>
-      <c r="M36" s="1"/>
-      <c r="N36" s="1"/>
-      <c r="O36" s="1">
+      <c r="Z36" s="1">
+        <v>4</v>
+      </c>
+      <c r="AA36" s="1"/>
+      <c r="AC36" s="1">
         <v>5</v>
       </c>
-      <c r="P36" s="1">
+      <c r="AD36" s="1">
         <v>5</v>
       </c>
-      <c r="Q36" s="1">
+      <c r="AE36" s="1">
         <v>5</v>
       </c>
-      <c r="R36" s="1"/>
-      <c r="S36" s="1"/>
-      <c r="T36" s="1">
+      <c r="AF36" s="1">
+        <v>5</v>
+      </c>
+      <c r="AG36" s="1"/>
+      <c r="AH36" s="1"/>
+      <c r="AI36" s="1">
         <v>6</v>
       </c>
-      <c r="U36" s="1">
+      <c r="AJ36" s="1">
         <v>6</v>
       </c>
-      <c r="V36" s="1">
+      <c r="AK36" s="1">
         <v>6</v>
       </c>
-      <c r="W36" s="1"/>
-      <c r="X36" s="1"/>
-      <c r="Y36" s="1">
-        <v>7</v>
-      </c>
-      <c r="Z36" s="1">
-        <v>7</v>
-      </c>
-      <c r="AA36" s="1">
-        <v>7</v>
-      </c>
-      <c r="AB36" s="1"/>
-      <c r="AC36" s="1"/>
-      <c r="AD36" s="1"/>
-      <c r="AE36" s="15"/>
-    </row>
-    <row r="37" spans="2:31">
+      <c r="AL36" s="1">
+        <v>6</v>
+      </c>
+      <c r="AM36" s="1"/>
+      <c r="AN36" s="1"/>
+      <c r="AO36" s="15"/>
+    </row>
+    <row r="37" spans="2:41">
       <c r="B37" s="14"/>
-      <c r="C37" s="30">
-        <v>2</v>
-      </c>
+      <c r="C37" s="30"/>
       <c r="AD37" s="1"/>
-      <c r="AE37" s="15"/>
-    </row>
-    <row r="38" spans="2:31">
+      <c r="AE37" s="1"/>
+      <c r="AF37" s="1"/>
+      <c r="AG37" s="1"/>
+      <c r="AH37" s="1"/>
+      <c r="AI37" s="1"/>
+      <c r="AJ37" s="1"/>
+      <c r="AK37" s="1"/>
+      <c r="AL37" s="1"/>
+      <c r="AM37" s="1"/>
+      <c r="AN37" s="1"/>
+      <c r="AO37" s="15"/>
+    </row>
+    <row r="38" spans="2:41">
       <c r="B38" s="14"/>
-      <c r="C38" s="1">
-        <v>2</v>
-      </c>
-      <c r="D38" s="1">
-        <v>2</v>
-      </c>
-      <c r="E38" s="1">
-        <v>2</v>
-      </c>
-      <c r="F38" s="1">
-        <v>2</v>
-      </c>
-      <c r="G38" s="1">
-        <v>2</v>
-      </c>
-      <c r="H38" s="1">
-        <v>2</v>
-      </c>
-      <c r="I38" s="1">
-        <v>2</v>
-      </c>
-      <c r="J38" s="1">
-        <v>2</v>
-      </c>
-      <c r="K38" s="1">
-        <v>2</v>
-      </c>
-      <c r="L38" s="1">
-        <v>2</v>
-      </c>
-      <c r="M38" s="1">
-        <v>2</v>
-      </c>
-      <c r="N38" s="1">
-        <v>2</v>
-      </c>
-      <c r="O38" s="1">
-        <v>2</v>
-      </c>
-      <c r="P38" s="1">
-        <v>2</v>
-      </c>
-      <c r="Q38" s="1">
-        <v>2</v>
-      </c>
-      <c r="R38" s="1">
-        <v>2</v>
-      </c>
-      <c r="S38" s="1">
-        <v>2</v>
-      </c>
-      <c r="T38" s="1">
-        <v>2</v>
-      </c>
-      <c r="U38" s="1">
-        <v>2</v>
-      </c>
-      <c r="V38" s="1">
-        <v>2</v>
-      </c>
-      <c r="W38" s="1">
-        <v>2</v>
-      </c>
-      <c r="X38" s="1">
-        <v>2</v>
-      </c>
-      <c r="Y38" s="1">
-        <v>2</v>
-      </c>
-      <c r="Z38" s="1">
-        <v>2</v>
-      </c>
-      <c r="AA38" s="1">
-        <v>2</v>
-      </c>
-      <c r="AB38" s="1">
-        <v>2</v>
-      </c>
-      <c r="AC38" s="1">
-        <v>2</v>
-      </c>
-      <c r="AD38" s="1">
-        <v>2</v>
-      </c>
-      <c r="AE38" s="15"/>
-    </row>
-    <row r="39" spans="2:31">
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+      <c r="L38" s="1"/>
+      <c r="M38" s="1"/>
+      <c r="N38" s="1"/>
+      <c r="O38" s="1"/>
+      <c r="P38" s="1"/>
+      <c r="Q38" s="1"/>
+      <c r="R38" s="1"/>
+      <c r="S38" s="1"/>
+      <c r="T38" s="1"/>
+      <c r="U38" s="1"/>
+      <c r="V38" s="1"/>
+      <c r="W38" s="1"/>
+      <c r="X38" s="1"/>
+      <c r="Y38" s="1"/>
+      <c r="Z38" s="1"/>
+      <c r="AA38" s="1"/>
+      <c r="AB38" s="1"/>
+      <c r="AC38" s="1"/>
+      <c r="AD38" s="1"/>
+      <c r="AE38" s="1"/>
+      <c r="AF38" s="1"/>
+      <c r="AG38" s="1"/>
+      <c r="AH38" s="1"/>
+      <c r="AI38" s="1"/>
+      <c r="AJ38" s="1"/>
+      <c r="AK38" s="1"/>
+      <c r="AL38" s="1"/>
+      <c r="AM38" s="1"/>
+      <c r="AN38" s="1"/>
+      <c r="AO38" s="15"/>
+    </row>
+    <row r="39" spans="2:41">
       <c r="B39" s="14"/>
       <c r="AD39" s="1"/>
-      <c r="AE39" s="15"/>
-    </row>
-    <row r="40" spans="2:31" ht="17" thickBot="1">
+      <c r="AE39" s="1"/>
+      <c r="AF39" s="1"/>
+      <c r="AG39" s="1"/>
+      <c r="AH39" s="1"/>
+      <c r="AI39" s="1"/>
+      <c r="AJ39" s="1"/>
+      <c r="AK39" s="1"/>
+      <c r="AL39" s="1"/>
+      <c r="AM39" s="1"/>
+      <c r="AN39" s="1"/>
+      <c r="AO39" s="15"/>
+    </row>
+    <row r="40" spans="2:41" ht="17" thickBot="1">
       <c r="B40" s="16"/>
       <c r="C40" s="17"/>
       <c r="D40" s="17"/>
@@ -7583,18 +8118,28 @@
       <c r="AB40" s="17"/>
       <c r="AC40" s="17"/>
       <c r="AD40" s="17"/>
-      <c r="AE40" s="18"/>
+      <c r="AE40" s="17"/>
+      <c r="AF40" s="17"/>
+      <c r="AG40" s="17"/>
+      <c r="AH40" s="17"/>
+      <c r="AI40" s="17"/>
+      <c r="AJ40" s="17"/>
+      <c r="AK40" s="17"/>
+      <c r="AL40" s="17"/>
+      <c r="AM40" s="17"/>
+      <c r="AN40" s="17"/>
+      <c r="AO40" s="18"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B1:AE40">
-    <cfRule type="cellIs" dxfId="90" priority="27" operator="equal">
-      <formula>3</formula>
+  <conditionalFormatting sqref="B1:AO3 B37:AO40 B11:I36 K11:O36 R11:AH11 U20:U36 U12:AC19 Q12:T36 W20:AA36 AC20:AO36 AE12:AH19 B4:AH10 AI4:AO19">
+    <cfRule type="cellIs" dxfId="90" priority="1" operator="equal">
+      <formula>2</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="89" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="88" priority="1" operator="equal">
-      <formula>2</formula>
+    <cfRule type="cellIs" dxfId="88" priority="27" operator="equal">
+      <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -7606,7 +8151,7 @@
   <dimension ref="A1:BL120"/>
   <sheetViews>
     <sheetView topLeftCell="R1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="Z77" sqref="Z77"/>
+      <selection activeCell="W1" sqref="W1:BJ1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -12204,7 +12749,7 @@
   <dimension ref="B1:BL120"/>
   <sheetViews>
     <sheetView zoomScale="20" zoomScaleNormal="20" workbookViewId="0">
-      <selection activeCell="AC21" sqref="AC21"/>
+      <selection activeCell="AC4" sqref="AC4:AR19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -16387,7 +16932,7 @@
   <dimension ref="A1:BL120"/>
   <sheetViews>
     <sheetView topLeftCell="J1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="BI22" sqref="BI22"/>
+      <selection activeCell="AC21" sqref="AC21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>